<commit_message>
Release: sfuse (v0.0.2) v3
</commit_message>
<xml_diff>
--- a/benchmark/result.xlsx
+++ b/benchmark/result.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Documents\github\SFUSE\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B33988-9E0D-4016-910B-2B8B9CCB57E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087AF176-9CBD-49AA-9EB3-D84131FBCFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{57B5C972-2613-42CF-A18C-E4DB28462054}"/>
+    <workbookView xWindow="-255" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="552" xr2:uid="{57B5C972-2613-42CF-A18C-E4DB28462054}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$X$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>워크로드</t>
   </si>
@@ -100,12 +100,40 @@
   <si>
     <t>66.1k</t>
   </si>
+  <si>
+    <t>BW (MiB/s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순차 쓰기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순차 읽기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>랜덤 쓰기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>랜덤 읽기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균 지연 (µs)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실행 시간 (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +151,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -178,21 +214,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -218,19 +239,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -306,6 +314,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -316,50 +350,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -367,6 +401,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4EA72E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2003,6 +2042,1277 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>BW (MiB/s)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SFUSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4EA72E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>순차 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>순차 읽기</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>랜덤 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>랜덤 읽기</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>190</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E11-4FD6-9939-2B91AF25FC22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ext4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>순차 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>순차 읽기</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>랜덤 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>랜덤 읽기</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>258</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E11-4FD6-9939-2B91AF25FC22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:axId val="333464511"/>
+        <c:axId val="333457791"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="333464511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333457791"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="333457791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333464511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US"/>
+              <a:t>평균 지연 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>(µs)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SFUSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4EA72E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>순차 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>순차 읽기</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>랜덤 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>랜덤 읽기</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$5:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3085</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2248</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC39-4B58-825A-FB566B165036}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ext4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>순차 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>순차 읽기</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>랜덤 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>랜덤 읽기</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$6:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2319</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>241</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC39-4B58-825A-FB566B165036}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:axId val="333489951"/>
+        <c:axId val="333490911"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="333489951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333490911"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="333490911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333489951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US"/>
+              <a:t>실행 시간 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>(ms)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SFUSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4EA72E"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>순차 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>순차 읽기</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>랜덤 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>랜덤 읽기</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$7:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C11A-42EE-8952-79730C2A5743}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ext4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>순차 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>순차 읽기</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>랜덤 쓰기</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>랜덤 읽기</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$8:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C11A-42EE-8952-79730C2A5743}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:axId val="333367071"/>
+        <c:axId val="333369951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="333367071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333369951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="333369951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333367071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2163,6 +3473,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3673,6 +5103,1515 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4180,15 +7119,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4472</xdr:colOff>
+      <xdr:colOff>10187</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>157535</xdr:rowOff>
+      <xdr:rowOff>163249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>337682</xdr:colOff>
+      <xdr:colOff>249767</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>116453</xdr:rowOff>
+      <xdr:rowOff>129719</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4216,15 +7155,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>556262</xdr:colOff>
+      <xdr:colOff>548641</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>169627</xdr:rowOff>
+      <xdr:rowOff>169625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>162804</xdr:colOff>
+      <xdr:colOff>80906</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>117115</xdr:rowOff>
+      <xdr:rowOff>146351</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4235,7 +7174,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4252,15 +7193,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>22943</xdr:colOff>
+      <xdr:colOff>15323</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>51104</xdr:rowOff>
+      <xdr:rowOff>58724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>365522</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>198699</xdr:rowOff>
+      <xdr:colOff>252998</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>18749</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4285,18 +7226,18 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>512943</xdr:colOff>
+      <xdr:colOff>512939</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>58062</xdr:rowOff>
+      <xdr:rowOff>59967</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>126681</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>211372</xdr:rowOff>
+      <xdr:colOff>60484</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>16913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4304,6 +7245,44 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A48C5DD4-1F83-09BE-47D6-5239D7A3E3BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>313877</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>131894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>543485</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>187587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="차트 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58F07404-0E59-A366-E302-C2329ADEF12C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4315,7 +7294,79 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22567</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>158378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>553124</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>214072</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="차트 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989DD2AE-F81C-1795-5DE4-0BFB8A0D3D57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>310285</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>98764</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542373</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>157410</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="차트 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB22F177-BDBF-5C74-7A07-9C2B3CBCC062}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4641,82 +7692,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742175E8-F3DC-4AAF-A3B7-49840553C637}">
-  <dimension ref="B1:I10"/>
+  <dimension ref="B1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V40" sqref="V40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.19921875" customWidth="1"/>
     <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" customWidth="1"/>
     <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.59765625" customWidth="1"/>
     <col min="8" max="8" width="5.69921875" customWidth="1"/>
     <col min="9" max="9" width="17.19921875" customWidth="1"/>
+    <col min="12" max="12" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="9" t="s">
+    <row r="1" spans="2:17" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:17" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="L2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>322</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>3085</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>311</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>321</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="4">
         <v>650.9</v>
       </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="3">
+        <v>322</v>
+      </c>
+      <c r="O3" s="3">
+        <v>441</v>
+      </c>
+      <c r="P3" s="3">
+        <v>121</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>190</v>
+      </c>
     </row>
-    <row r="4" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
+    <row r="4" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -4738,37 +7826,69 @@
       <c r="I4" s="2">
         <v>142</v>
       </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="1">
+        <v>429</v>
+      </c>
+      <c r="O4" s="1">
+        <v>469</v>
+      </c>
+      <c r="P4" s="1">
+        <v>135</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>258</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>441</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>2248</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>227</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>440</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="4">
         <v>828.7</v>
       </c>
+      <c r="L5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="3">
+        <v>3085</v>
+      </c>
+      <c r="O5" s="3">
+        <v>2248</v>
+      </c>
+      <c r="P5" s="3">
+        <v>516</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>327</v>
+      </c>
     </row>
-    <row r="6" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="13" t="s">
-        <v>12</v>
-      </c>
+    <row r="6" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -4790,37 +7910,69 @@
       <c r="I6" s="2">
         <v>101.8</v>
       </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="1">
+        <v>2319</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2114</v>
+      </c>
+      <c r="P6" s="1">
+        <v>461</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>241</v>
+      </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>121</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>516</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>829</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="4">
         <v>85.6</v>
       </c>
+      <c r="L7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="3">
+        <v>311</v>
+      </c>
+      <c r="O7" s="3">
+        <v>227</v>
+      </c>
+      <c r="P7" s="3">
+        <v>829</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>525</v>
+      </c>
     </row>
-    <row r="8" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="15" t="s">
-        <v>13</v>
-      </c>
+    <row r="8" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="13"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -4842,37 +7994,51 @@
       <c r="I8" s="2">
         <v>707.3</v>
       </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="1">
+        <v>233</v>
+      </c>
+      <c r="O8" s="1">
+        <v>213</v>
+      </c>
+      <c r="P8" s="1">
+        <v>740</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>387</v>
+      </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>190</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>327</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>525</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="4">
         <v>77.900000000000006</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="10" spans="2:17" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="15"/>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
@@ -4896,9 +8062,21 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L7:L8"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="38" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>